<commit_message>
Update 14.11. & Ne
</commit_message>
<xml_diff>
--- a/Teile.xlsx
+++ b/Teile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Drohne" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="154">
   <si>
     <t>Preis</t>
   </si>
@@ -473,6 +473,24 @@
   </si>
   <si>
     <t>Breadboards</t>
+  </si>
+  <si>
+    <t>Helfende Hand</t>
+  </si>
+  <si>
+    <t>Babymax</t>
+  </si>
+  <si>
+    <t>Lot (Flüssig)</t>
+  </si>
+  <si>
+    <t>CFH Elekroniklot</t>
+  </si>
+  <si>
+    <t>Lötkolben set</t>
+  </si>
+  <si>
+    <t>Soldering Iron</t>
   </si>
 </sst>
 </file>
@@ -523,7 +541,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -538,6 +556,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -583,7 +613,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -602,9 +632,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Eingabe" xfId="3" builtinId="20"/>
@@ -940,21 +977,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
     <col min="7" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -963,7 +1000,7 @@
       </c>
       <c r="D1" s="1">
         <f>SUM(D4:D38)</f>
-        <v>289.08</v>
+        <v>337.40999999999997</v>
       </c>
       <c r="E1" s="2">
         <f>SUM(E4:E38)</f>
@@ -979,7 +1016,7 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="K2" t="s">
         <v>95</v>
       </c>
@@ -991,7 +1028,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1027,7 +1064,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>28</v>
       </c>
@@ -1052,7 +1089,7 @@
         <v>43032</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
@@ -1078,8 +1115,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="10">
@@ -1104,8 +1141,8 @@
         <v>43042</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
         <v>121</v>
       </c>
       <c r="B7" s="10">
@@ -1124,8 +1161,8 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
         <v>140</v>
       </c>
       <c r="B8" s="10">
@@ -1147,7 +1184,7 @@
         <v>43042</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>31</v>
       </c>
@@ -1174,7 +1211,7 @@
         <v>43042</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>147</v>
       </c>
@@ -1185,7 +1222,7 @@
         <v>43042</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>30</v>
       </c>
@@ -1207,7 +1244,7 @@
         <v>43043</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>67</v>
       </c>
@@ -1230,7 +1267,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>146</v>
       </c>
@@ -1244,7 +1281,7 @@
         <v>43043</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>3</v>
       </c>
@@ -1274,7 +1311,7 @@
         <v>43045</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>63</v>
       </c>
@@ -1294,7 +1331,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>66</v>
       </c>
@@ -1317,7 +1354,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>73</v>
       </c>
@@ -1337,7 +1374,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>118</v>
       </c>
@@ -1354,7 +1391,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>34</v>
       </c>
@@ -1377,7 +1414,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>135</v>
       </c>
@@ -1397,7 +1434,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>109</v>
       </c>
@@ -1420,7 +1457,7 @@
         <v>43050</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>103</v>
       </c>
@@ -1440,7 +1477,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>133</v>
       </c>
@@ -1460,8 +1497,8 @@
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="10">
@@ -1487,122 +1524,164 @@
         <v>0</v>
       </c>
       <c r="H24" s="13">
-        <v>43071</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>77</v>
+        <v>43053</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="B25" s="10">
         <v>1</v>
       </c>
-      <c r="C25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="6">
-        <v>10</v>
-      </c>
-      <c r="H25" s="13">
-        <v>43071</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" s="10">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="6">
-        <v>10.59</v>
-      </c>
-      <c r="H26" s="13">
-        <v>43071</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="10">
-        <v>1</v>
-      </c>
-      <c r="C27" t="str">
+      <c r="C25" t="str">
         <f>Höhe!B2</f>
         <v>MPL3115A2</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D25" s="8">
         <f>Höhe!C2</f>
         <v>4</v>
       </c>
-      <c r="F27">
+      <c r="F25">
         <f>Höhe!D2</f>
         <v>1</v>
       </c>
+      <c r="H25" s="13">
+        <v>43053</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="10">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1.35</v>
+      </c>
+      <c r="H26" s="13">
+        <v>43053</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" s="16">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27" s="6">
+        <v>3.33</v>
+      </c>
       <c r="H27" s="13">
-        <v>43096</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="B28" s="10">
+        <v>43055</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" s="16">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="D28" s="6">
-        <v>1.35</v>
+        <v>30</v>
       </c>
       <c r="H28" s="13">
-        <v>43096</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+        <v>43055</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="10">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>149</v>
+      </c>
+      <c r="D29" s="6">
+        <v>15</v>
+      </c>
+      <c r="H29" s="13">
+        <v>43059</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="10">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="6">
+        <v>10</v>
+      </c>
+      <c r="H30" s="13">
+        <v>43071</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="10">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="6">
+        <v>10.59</v>
+      </c>
+      <c r="H31" s="13">
+        <v>43071</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="10">
-        <v>1</v>
-      </c>
-      <c r="D29" s="6">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
+      <c r="B32" s="10">
+        <v>1</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
         <v>200</v>
       </c>
-      <c r="H29" s="13"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D30" s="6"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D31" s="6"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D32" s="6"/>
+      <c r="H32" s="13"/>
     </row>
   </sheetData>
-  <sortState ref="A4:I30">
-    <sortCondition ref="H4:H30"/>
+  <sortState ref="A4:I32">
+    <sortCondition ref="H4:H32"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="I15" r:id="rId1"/>
@@ -1610,10 +1689,10 @@
     <hyperlink ref="I12" r:id="rId3"/>
     <hyperlink ref="I17" r:id="rId4"/>
     <hyperlink ref="I19" r:id="rId5"/>
-    <hyperlink ref="I25" r:id="rId6"/>
+    <hyperlink ref="I30" r:id="rId6"/>
     <hyperlink ref="I5" r:id="rId7"/>
-    <hyperlink ref="I26" r:id="rId8"/>
-    <hyperlink ref="I28" r:id="rId9"/>
+    <hyperlink ref="I31" r:id="rId8"/>
+    <hyperlink ref="I26" r:id="rId9"/>
     <hyperlink ref="I18" r:id="rId10"/>
     <hyperlink ref="I23" r:id="rId11"/>
     <hyperlink ref="I7" r:id="rId12"/>
@@ -1632,13 +1711,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1655,7 +1734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>113</v>
       </c>
@@ -1685,14 +1764,14 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>142</v>
       </c>
@@ -1700,7 +1779,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -1708,7 +1787,7 @@
         <v>82.52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>143</v>
       </c>
@@ -1716,7 +1795,7 @@
         <v>31.28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>144</v>
       </c>
@@ -1728,7 +1807,7 @@
         <v>290.14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -1749,12 +1828,12 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1774,7 +1853,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -1791,7 +1870,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -1811,7 +1890,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -1828,7 +1907,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" s="8"/>
     </row>
   </sheetData>
@@ -1852,9 +1931,9 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1880,7 +1959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -1907,7 +1986,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>1</v>
       </c>
@@ -1941,14 +2020,14 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="6" max="7" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="6" max="7" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1980,7 +2059,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2014,7 +2093,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2048,7 +2127,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -2080,7 +2159,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="b">
         <v>0</v>
       </c>
@@ -2112,7 +2191,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
         <v>0</v>
       </c>
@@ -2144,7 +2223,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -2178,7 +2257,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="b">
         <v>0</v>
       </c>
@@ -2209,7 +2288,7 @@
         <v>10.83916083916084</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C9" s="4"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2220,7 +2299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C10" s="4"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2231,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C11" s="4"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2242,7 +2321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C12" s="4"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -2253,7 +2332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>46</v>
       </c>
@@ -2265,138 +2344,138 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C14" s="4"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C15" s="4"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C16" s="4"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C17" s="4"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C18" s="4"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C19" s="4"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C20" s="4"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C21" s="4"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C22" s="4"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C23" s="4"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C24" s="4"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C25" s="4"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C26" s="4"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C27" s="4"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C39" s="4"/>
     </row>
   </sheetData>
@@ -2424,13 +2503,13 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2459,7 +2538,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2485,7 +2564,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2511,7 +2590,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -2538,7 +2617,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="b">
         <v>0</v>
       </c>
@@ -2558,7 +2637,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
         <v>0</v>
       </c>
@@ -2578,7 +2657,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -2604,7 +2683,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I24" t="s">
         <v>126</v>
       </c>
@@ -2612,7 +2691,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I25" t="s">
         <v>127</v>
       </c>
@@ -2648,9 +2727,9 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2667,7 +2746,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2681,7 +2760,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2698,7 +2777,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -2712,37 +2791,37 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" s="8"/>
     </row>
   </sheetData>
@@ -2765,13 +2844,13 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2791,7 +2870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2811,7 +2890,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C3" s="8">
         <v>3</v>
       </c>
@@ -2822,70 +2901,70 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C25" s="8"/>
     </row>
   </sheetData>
@@ -2905,9 +2984,9 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2924,7 +3003,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2957,12 +3036,12 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2985,7 +3064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3005,7 +3084,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Ultraschalll, GPS und Höhensensor
</commit_message>
<xml_diff>
--- a/Teile.xlsx
+++ b/Teile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Drohne" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="164">
   <si>
     <t>Preis</t>
   </si>
@@ -503,6 +503,24 @@
   </si>
   <si>
     <t>5 16*10cm</t>
+  </si>
+  <si>
+    <t>GPS 2</t>
+  </si>
+  <si>
+    <t>Ultraschall</t>
+  </si>
+  <si>
+    <t>BMP180</t>
+  </si>
+  <si>
+    <t>https://www.ebay.de/itm/252715059842</t>
+  </si>
+  <si>
+    <t>https://www.ebay.de/itm/162571876188</t>
+  </si>
+  <si>
+    <t>https://www.ebay.de/itm/162675931015</t>
   </si>
 </sst>
 </file>
@@ -959,23 +977,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
     <col min="7" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -984,7 +1002,7 @@
       </c>
       <c r="D1" s="1">
         <f>SUM(D4:D38)</f>
-        <v>355.98999999999995</v>
+        <v>373.72999999999996</v>
       </c>
       <c r="E1" s="2">
         <f>SUM(E4:E38)</f>
@@ -1000,7 +1018,7 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="K2" t="s">
         <v>95</v>
       </c>
@@ -1012,7 +1030,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1048,7 +1066,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>28</v>
       </c>
@@ -1073,7 +1091,7 @@
         <v>43032</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
@@ -1099,7 +1117,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>32</v>
       </c>
@@ -1125,7 +1143,7 @@
         <v>43042</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>121</v>
       </c>
@@ -1146,7 +1164,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>140</v>
       </c>
@@ -1169,7 +1187,7 @@
         <v>43042</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>31</v>
       </c>
@@ -1196,7 +1214,7 @@
         <v>43042</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>147</v>
       </c>
@@ -1207,7 +1225,7 @@
         <v>43042</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>30</v>
       </c>
@@ -1229,7 +1247,7 @@
         <v>43043</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>67</v>
       </c>
@@ -1252,7 +1270,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>146</v>
       </c>
@@ -1266,7 +1284,7 @@
         <v>43043</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>3</v>
       </c>
@@ -1296,7 +1314,7 @@
         <v>43045</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>63</v>
       </c>
@@ -1316,7 +1334,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>66</v>
       </c>
@@ -1339,7 +1357,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>73</v>
       </c>
@@ -1359,7 +1377,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>118</v>
       </c>
@@ -1376,7 +1394,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>34</v>
       </c>
@@ -1399,7 +1417,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>135</v>
       </c>
@@ -1419,7 +1437,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>109</v>
       </c>
@@ -1442,7 +1460,7 @@
         <v>43050</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>103</v>
       </c>
@@ -1462,7 +1480,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>133</v>
       </c>
@@ -1482,7 +1500,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>2</v>
       </c>
@@ -1512,7 +1530,7 @@
         <v>43053</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>35</v>
       </c>
@@ -1535,7 +1553,7 @@
         <v>43053</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>108</v>
       </c>
@@ -1555,7 +1573,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>150</v>
       </c>
@@ -1572,7 +1590,7 @@
         <v>43055</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>152</v>
       </c>
@@ -1589,7 +1607,7 @@
         <v>43055</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>77</v>
       </c>
@@ -1609,7 +1627,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
         <v>148</v>
       </c>
@@ -1626,7 +1644,7 @@
         <v>43056</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
         <v>86</v>
       </c>
@@ -1646,7 +1664,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
         <v>29</v>
       </c>
@@ -1664,7 +1682,7 @@
       </c>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>154</v>
       </c>
@@ -1687,7 +1705,7 @@
         <v>43077</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>156</v>
       </c>
@@ -1705,6 +1723,66 @@
       </c>
       <c r="H34" s="13">
         <v>43071</v>
+      </c>
+      <c r="I34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B35" s="15">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="6">
+        <v>11</v>
+      </c>
+      <c r="H35" s="13">
+        <v>43081</v>
+      </c>
+      <c r="I35" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B36" s="15">
+        <v>1</v>
+      </c>
+      <c r="D36" s="6">
+        <v>2.85</v>
+      </c>
+      <c r="H36" s="13">
+        <v>43081</v>
+      </c>
+      <c r="I36" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="15">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>160</v>
+      </c>
+      <c r="D37" s="6">
+        <v>3.89</v>
+      </c>
+      <c r="H37" s="13">
+        <v>43080</v>
+      </c>
+      <c r="I37" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1739,13 +1817,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1762,7 +1840,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>113</v>
       </c>
@@ -1792,14 +1870,14 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>142</v>
       </c>
@@ -1807,7 +1885,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -1815,7 +1893,7 @@
         <v>82.52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>143</v>
       </c>
@@ -1823,7 +1901,7 @@
         <v>31.28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>144</v>
       </c>
@@ -1835,7 +1913,7 @@
         <v>290.14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -1856,12 +1934,12 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1881,7 +1959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -1898,7 +1976,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -1918,7 +1996,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -1935,7 +2013,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" s="8"/>
     </row>
   </sheetData>
@@ -1959,9 +2037,9 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1987,7 +2065,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2014,7 +2092,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>1</v>
       </c>
@@ -2048,14 +2126,14 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="6" max="7" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="6" max="7" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2087,7 +2165,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2121,7 +2199,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2155,7 +2233,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -2187,7 +2265,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="b">
         <v>0</v>
       </c>
@@ -2219,7 +2297,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
         <v>0</v>
       </c>
@@ -2251,7 +2329,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -2285,7 +2363,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="b">
         <v>0</v>
       </c>
@@ -2316,7 +2394,7 @@
         <v>10.83916083916084</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C9" s="4"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2327,7 +2405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C10" s="4"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2338,7 +2416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C11" s="4"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2349,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C12" s="4"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -2360,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>46</v>
       </c>
@@ -2372,138 +2450,138 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C14" s="4"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C15" s="4"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C16" s="4"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C17" s="4"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C18" s="4"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C19" s="4"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C20" s="4"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C21" s="4"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C22" s="4"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C23" s="4"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C24" s="4"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C25" s="4"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C26" s="4"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C27" s="4"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C39" s="4"/>
     </row>
   </sheetData>
@@ -2531,13 +2609,13 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2566,7 +2644,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2592,7 +2670,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2618,7 +2696,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -2645,7 +2723,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="b">
         <v>0</v>
       </c>
@@ -2665,7 +2743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
         <v>0</v>
       </c>
@@ -2685,7 +2763,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -2711,7 +2789,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I24" t="s">
         <v>126</v>
       </c>
@@ -2719,7 +2797,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I25" t="s">
         <v>127</v>
       </c>
@@ -2755,9 +2833,9 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2774,7 +2852,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2788,7 +2866,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2805,7 +2883,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -2819,37 +2897,37 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" s="8"/>
     </row>
   </sheetData>
@@ -2872,13 +2950,13 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2898,7 +2976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2918,7 +2996,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C3" s="8">
         <v>3</v>
       </c>
@@ -2929,70 +3007,70 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C25" s="8"/>
     </row>
   </sheetData>
@@ -3012,9 +3090,9 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3031,7 +3109,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3064,12 +3142,12 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3092,7 +3170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3112,7 +3190,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Update 13.12. Alle Bestellungen abgeschlossen
</commit_message>
<xml_diff>
--- a/Teile.xlsx
+++ b/Teile.xlsx
@@ -979,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1665,64 +1665,63 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="10">
-        <v>1</v>
-      </c>
-      <c r="D32" s="6">
-        <v>0</v>
+      <c r="A32" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B32" s="15">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32" s="1">
+        <v>10</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
-      <c r="F32">
-        <v>200</v>
-      </c>
-      <c r="H32" s="13"/>
+      <c r="H32" s="13">
+        <v>43071</v>
+      </c>
+      <c r="I32" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
-        <v>154</v>
+      <c r="A33" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="B33" s="15">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>155</v>
-      </c>
-      <c r="D33" s="7">
-        <v>6.33</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
+        <v>160</v>
+      </c>
+      <c r="D33" s="6">
+        <v>3.89</v>
       </c>
       <c r="H33" s="13">
         <v>43077</v>
       </c>
+      <c r="I33" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B34" s="15">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>157</v>
-      </c>
-      <c r="D34" s="1">
-        <v>10</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
+        <v>88</v>
+      </c>
+      <c r="D34" s="6">
+        <v>11</v>
       </c>
       <c r="H34" s="13">
-        <v>43071</v>
+        <v>43080</v>
       </c>
       <c r="I34" t="s">
         <v>161</v>
@@ -1730,64 +1729,65 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B35" s="15">
         <v>1</v>
       </c>
-      <c r="C35" t="s">
-        <v>88</v>
-      </c>
       <c r="D35" s="6">
-        <v>11</v>
+        <v>2.85</v>
       </c>
       <c r="H35" s="13">
         <v>43080</v>
       </c>
       <c r="I35" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B36" s="15">
         <v>1</v>
       </c>
-      <c r="D36" s="6">
-        <v>2.85</v>
+      <c r="C36" t="s">
+        <v>155</v>
+      </c>
+      <c r="D36" s="7">
+        <v>6.33</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
       </c>
       <c r="H36" s="13">
-        <v>43080</v>
-      </c>
-      <c r="I36" t="s">
-        <v>162</v>
+        <v>43081</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="15">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>160</v>
+      <c r="A37" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="10">
+        <v>1</v>
       </c>
       <c r="D37" s="6">
-        <v>3.89</v>
-      </c>
-      <c r="H37" s="13">
-        <v>43077</v>
-      </c>
-      <c r="I37" t="s">
-        <v>163</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>200</v>
+      </c>
+      <c r="H37" s="13"/>
     </row>
   </sheetData>
-  <sortState ref="A4:I32">
-    <sortCondition ref="H4:H32"/>
+  <sortState ref="A5:I37">
+    <sortCondition ref="H5:H37"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="I15" r:id="rId1"/>

</xml_diff>

<commit_message>
Raspberry pi 3 bestellt
</commit_message>
<xml_diff>
--- a/Teile.xlsx
+++ b/Teile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Drohne" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="169">
   <si>
     <t>Preis</t>
   </si>
@@ -524,6 +524,18 @@
   </si>
   <si>
     <t>https://www.ebay.de/itm/HC-SR04-Ultraschall-Sensor-Modul-Entfernungsmesser-Arduino-Raspberry-Pi/252715059842?ssPageName=STRK%3AMEBIDX%3AIT&amp;_trksid=p2057872.m2749.l2649</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 3</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/Raspberry-Pi-Official-Desktop-Starter/dp/B01CI5879A/ref=cm_cr_arp_d_product_top?ie=UTF8</t>
+  </si>
+  <si>
+    <t>Schutzkappen</t>
+  </si>
+  <si>
+    <t>jst-xh 3s kopfschutz</t>
   </si>
 </sst>
 </file>
@@ -574,7 +586,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -589,6 +601,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -623,7 +641,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -647,6 +665,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Eingabe" xfId="3" builtinId="20"/>
@@ -980,23 +999,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
     <col min="7" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1005,7 +1024,7 @@
       </c>
       <c r="D1" s="1">
         <f>SUM(D4:D38)</f>
-        <v>373.72999999999996</v>
+        <v>424.72999999999996</v>
       </c>
       <c r="E1" s="2">
         <f>SUM(E4:E38)</f>
@@ -1021,7 +1040,7 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="K2" t="s">
         <v>95</v>
       </c>
@@ -1033,7 +1052,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1069,7 +1088,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>28</v>
       </c>
@@ -1094,7 +1113,7 @@
         <v>43032</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
@@ -1120,7 +1139,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>32</v>
       </c>
@@ -1146,7 +1165,7 @@
         <v>43042</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>121</v>
       </c>
@@ -1167,7 +1186,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>140</v>
       </c>
@@ -1190,7 +1209,7 @@
         <v>43042</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>31</v>
       </c>
@@ -1217,7 +1236,7 @@
         <v>43042</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>147</v>
       </c>
@@ -1228,7 +1247,7 @@
         <v>43042</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>30</v>
       </c>
@@ -1250,7 +1269,7 @@
         <v>43043</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>67</v>
       </c>
@@ -1273,7 +1292,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>146</v>
       </c>
@@ -1287,7 +1306,7 @@
         <v>43043</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>3</v>
       </c>
@@ -1317,7 +1336,7 @@
         <v>43045</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>63</v>
       </c>
@@ -1337,7 +1356,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>66</v>
       </c>
@@ -1360,7 +1379,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>73</v>
       </c>
@@ -1380,7 +1399,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>118</v>
       </c>
@@ -1397,7 +1416,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>34</v>
       </c>
@@ -1420,7 +1439,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>135</v>
       </c>
@@ -1440,7 +1459,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>109</v>
       </c>
@@ -1463,7 +1482,7 @@
         <v>43050</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>103</v>
       </c>
@@ -1483,7 +1502,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>133</v>
       </c>
@@ -1503,7 +1522,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>2</v>
       </c>
@@ -1533,7 +1552,7 @@
         <v>43053</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>35</v>
       </c>
@@ -1556,7 +1575,7 @@
         <v>43053</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>108</v>
       </c>
@@ -1576,7 +1595,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>150</v>
       </c>
@@ -1593,7 +1612,7 @@
         <v>43055</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>152</v>
       </c>
@@ -1610,7 +1629,7 @@
         <v>43055</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>77</v>
       </c>
@@ -1630,7 +1649,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
         <v>148</v>
       </c>
@@ -1647,7 +1666,7 @@
         <v>43056</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
         <v>86</v>
       </c>
@@ -1667,7 +1686,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
         <v>156</v>
       </c>
@@ -1690,7 +1709,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
         <v>35</v>
       </c>
@@ -1710,7 +1729,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>158</v>
       </c>
@@ -1730,7 +1749,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
         <v>159</v>
       </c>
@@ -1747,7 +1766,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
         <v>154</v>
       </c>
@@ -1770,7 +1789,7 @@
         <v>43081</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
         <v>29</v>
       </c>
@@ -1787,6 +1806,40 @@
         <v>200</v>
       </c>
       <c r="H37" s="13"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B38" s="15">
+        <v>1</v>
+      </c>
+      <c r="D38" s="6">
+        <v>51</v>
+      </c>
+      <c r="H38" s="13">
+        <v>43105</v>
+      </c>
+      <c r="I38" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" s="15">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>168</v>
+      </c>
+      <c r="D39" s="6">
+        <v>2.35</v>
+      </c>
+      <c r="H39" s="13">
+        <v>43164</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A5:I37">
@@ -1823,13 +1876,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1846,7 +1899,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>113</v>
       </c>
@@ -1876,14 +1929,14 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>142</v>
       </c>
@@ -1891,7 +1944,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -1899,7 +1952,7 @@
         <v>82.52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>143</v>
       </c>
@@ -1907,7 +1960,7 @@
         <v>31.28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>144</v>
       </c>
@@ -1919,7 +1972,7 @@
         <v>290.14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -1940,12 +1993,12 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1965,7 +2018,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -1982,7 +2035,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2002,7 +2055,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -2019,7 +2072,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" s="8"/>
     </row>
   </sheetData>
@@ -2043,9 +2096,9 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2071,7 +2124,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2098,7 +2151,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>1</v>
       </c>
@@ -2132,14 +2185,14 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="6" max="7" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="6" max="7" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2171,7 +2224,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2205,7 +2258,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2239,7 +2292,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -2271,7 +2324,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="b">
         <v>0</v>
       </c>
@@ -2303,7 +2356,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
         <v>0</v>
       </c>
@@ -2335,7 +2388,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -2369,7 +2422,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="b">
         <v>0</v>
       </c>
@@ -2400,7 +2453,7 @@
         <v>10.83916083916084</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C9" s="4"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2411,7 +2464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C10" s="4"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2422,7 +2475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C11" s="4"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2433,7 +2486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C12" s="4"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -2444,7 +2497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>46</v>
       </c>
@@ -2456,138 +2509,138 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C14" s="4"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C15" s="4"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C16" s="4"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C17" s="4"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C18" s="4"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C19" s="4"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C20" s="4"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C21" s="4"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C22" s="4"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C23" s="4"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C24" s="4"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C25" s="4"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C26" s="4"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C27" s="4"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C39" s="4"/>
     </row>
   </sheetData>
@@ -2615,13 +2668,13 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2650,7 +2703,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2676,7 +2729,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2702,7 +2755,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -2729,7 +2782,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="b">
         <v>0</v>
       </c>
@@ -2749,7 +2802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
         <v>0</v>
       </c>
@@ -2769,7 +2822,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -2795,7 +2848,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I24" t="s">
         <v>126</v>
       </c>
@@ -2803,7 +2856,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I25" t="s">
         <v>127</v>
       </c>
@@ -2839,9 +2892,9 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2858,7 +2911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2872,7 +2925,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -2889,7 +2942,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>0</v>
       </c>
@@ -2903,37 +2956,37 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" s="8"/>
     </row>
   </sheetData>
@@ -2956,13 +3009,13 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2982,7 +3035,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3002,7 +3055,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C3" s="8">
         <v>3</v>
       </c>
@@ -3013,70 +3066,70 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C25" s="8"/>
     </row>
   </sheetData>
@@ -3096,9 +3149,9 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3115,7 +3168,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3148,12 +3201,12 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3176,7 +3229,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -3196,7 +3249,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>0</v>
       </c>

</xml_diff>